<commit_message>
Completo - falta correcoes
</commit_message>
<xml_diff>
--- a/Customizados DW.xlsx
+++ b/Customizados DW.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhjae\Desktop\clientes\BRASANITAS\Customizados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhjae\Desktop\clientes\BRASANITAS\customizados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E336E0-8F25-46E5-8CC7-1326588E5DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC9C732-E6B8-4C74-ACBE-62D07B15F7E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7125" yWindow="1245" windowWidth="21675" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPROC" sheetId="1" r:id="rId1"/>
-    <sheet name="CPAR" sheetId="2" r:id="rId2"/>
+    <sheet name="Alterações" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>MSAF_LOAD_FILE_ECD_CPROC</t>
   </si>
@@ -120,6 +120,12 @@
 SAFX262 - Replicar dados de periodos anteriores.
 Carregar CSV de parametros de geracai do bloco K (Contas Detentoras, Contrapartidas e eliminações)
 Permitir geracao da SAFX262 atraves das aglutinacoes</t>
+  </si>
+  <si>
+    <t>Requisitos a serem atendidos Tax ONE</t>
+  </si>
+  <si>
+    <t>Horas</t>
   </si>
 </sst>
 </file>
@@ -570,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C08488A5-F6B4-4384-A6DF-1AABCE936A98}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,17 +734,19 @@
         <v>10</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>

</xml_diff>